<commit_message>
changes on html pages, added base for global html, broke export
</commit_message>
<xml_diff>
--- a/src/controle_horas_2025-06.xlsx
+++ b/src/controle_horas_2025-06.xlsx
@@ -39,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -59,11 +59,22 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -71,6 +82,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -436,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C3:N3"/>
+  <dimension ref="C3:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,6 +536,346 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Marlon Passeri</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>656</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4" t="n"/>
+      <c r="L4" s="4" t="n"/>
+      <c r="M4" s="4" t="n"/>
+      <c r="N4" s="7" t="n"/>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>Leonardo</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>1796</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="K5" s="4" t="n"/>
+      <c r="L5" s="4" t="n"/>
+      <c r="M5" s="4" t="n"/>
+      <c r="N5" s="7" t="n"/>
+    </row>
+    <row r="6">
+      <c r="C6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>Leonardo</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>1003</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K6" s="4" t="n"/>
+      <c r="L6" s="4" t="n"/>
+      <c r="M6" s="4" t="n"/>
+      <c r="N6" s="7" t="n"/>
+    </row>
+    <row r="7">
+      <c r="C7" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>Fel</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>2516</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4" t="n"/>
+      <c r="L7" s="4" t="n"/>
+      <c r="M7" s="4" t="n"/>
+      <c r="N7" s="7" t="n"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>Marlon Soares Passeri</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>1881</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4" t="n"/>
+      <c r="L8" s="4" t="n"/>
+      <c r="M8" s="4" t="n"/>
+      <c r="N8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="C9" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>Guilherme Fernandes</t>
+        </is>
+      </c>
+      <c r="F9" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>656</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>0.1230769230769231</v>
+      </c>
+      <c r="K9" s="4" t="n"/>
+      <c r="L9" s="4" t="n"/>
+      <c r="M9" s="4" t="n"/>
+      <c r="N9" s="7" t="n"/>
+    </row>
+    <row r="10">
+      <c r="C10" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>Guilherme Fernandes</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G10" s="5" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>669</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>0.1230769230769231</v>
+      </c>
+      <c r="K10" s="4" t="n"/>
+      <c r="L10" s="4" t="n"/>
+      <c r="M10" s="4" t="n"/>
+      <c r="N10" s="7" t="n"/>
+    </row>
+    <row r="11">
+      <c r="C11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>Guilherme Fernandes</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>1796</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="J11" s="6" t="n">
+        <v>0.4461538461538462</v>
+      </c>
+      <c r="K11" s="4" t="n"/>
+      <c r="L11" s="4" t="n"/>
+      <c r="M11" s="4" t="n"/>
+      <c r="N11" s="7" t="n"/>
+    </row>
+    <row r="12">
+      <c r="C12" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>Guilherme Fernandes</t>
+        </is>
+      </c>
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>3040</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="K12" s="4" t="n"/>
+      <c r="L12" s="4" t="n"/>
+      <c r="M12" s="4" t="n"/>
+      <c r="N12" s="7" t="n"/>
+    </row>
+    <row r="13">
+      <c r="C13" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>Guilherme Fernandes</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>2139</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="J13" s="6" t="n">
+        <v>0.2769230769230769</v>
+      </c>
+      <c r="K13" s="4" t="n"/>
+      <c r="L13" s="4" t="n"/>
+      <c r="M13" s="4" t="n"/>
+      <c r="N13" s="7" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de Titulos e CSS
</commit_message>
<xml_diff>
--- a/src/controle_horas_2025-06.xlsx
+++ b/src/controle_horas_2025-06.xlsx
@@ -39,7 +39,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -59,11 +59,22 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -71,6 +82,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -436,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C3:N3"/>
+  <dimension ref="C3:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,6 +536,40 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Marlon Passeri</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>2025-06</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>656</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4" t="n"/>
+      <c r="L4" s="4" t="n"/>
+      <c r="M4" s="4" t="n"/>
+      <c r="N4" s="7" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>